<commit_message>
fix: add shl integration
</commit_message>
<xml_diff>
--- a/static/handbalnl/programma.xlsx
+++ b/static/handbalnl/programma.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>Datum</t>
   </si>
@@ -177,6 +177,15 @@
   </si>
   <si>
     <t>12-10-2024</t>
+  </si>
+  <si>
+    <t>15-10-2024</t>
+  </si>
+  <si>
+    <t>20:30:00</t>
+  </si>
+  <si>
+    <t>16-10-2024</t>
   </si>
   <si>
     <t>19-10-2024</t>
@@ -1033,22 +1042,22 @@
         <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E16">
-        <v>584</v>
+        <v>616</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H16" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="I16"/>
     </row>
@@ -1060,22 +1069,22 @@
         <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E17">
-        <v>616</v>
+        <v>584</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="I17"/>
     </row>
@@ -1624,22 +1633,22 @@
         <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E38">
-        <v>1248</v>
+        <v>1397</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H38" t="s">
         <v>15</v>
@@ -1648,25 +1657,25 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B39" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E39">
-        <v>1367</v>
+        <v>1278</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -1675,52 +1684,52 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E40">
-        <v>1307</v>
+        <v>1248</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H40" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="I40"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E41">
-        <v>1336</v>
+        <v>1367</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H41" t="s">
         <v>15</v>
@@ -1729,52 +1738,52 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
         <v>24</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D42" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E42">
-        <v>1397</v>
+        <v>1307</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H42" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="I42"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B43" t="s">
         <v>24</v>
       </c>
       <c r="C43" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D43" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E43">
-        <v>1278</v>
+        <v>1336</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H43" t="s">
         <v>15</v>
@@ -1783,7 +1792,7 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -1810,7 +1819,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B45" t="s">
         <v>10</v>
@@ -1837,7 +1846,7 @@
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B46" t="s">
         <v>10</v>
@@ -1864,7 +1873,7 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B47" t="s">
         <v>24</v>
@@ -1891,25 +1900,25 @@
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B48" t="s">
         <v>24</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D48" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E48">
-        <v>1519</v>
+        <v>1456</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="H48" t="s">
         <v>15</v>
@@ -1918,25 +1927,25 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B49" t="s">
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D49" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E49">
-        <v>1456</v>
+        <v>1519</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H49" t="s">
         <v>15</v>
@@ -1945,7 +1954,7 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
@@ -1972,7 +1981,7 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B51" t="s">
         <v>24</v>
@@ -1999,7 +2008,7 @@
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B52" t="s">
         <v>24</v>
@@ -2026,7 +2035,7 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B53" t="s">
         <v>24</v>
@@ -2053,7 +2062,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>24</v>
@@ -2080,10 +2089,10 @@
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
         <v>33</v>
@@ -2107,7 +2116,7 @@
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
@@ -2134,7 +2143,7 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
@@ -2161,7 +2170,7 @@
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B58" t="s">
         <v>20</v>
@@ -2188,7 +2197,7 @@
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B59" t="s">
         <v>24</v>
@@ -2215,7 +2224,7 @@
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B60" t="s">
         <v>24</v>
@@ -2242,7 +2251,7 @@
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B61" t="s">
         <v>24</v>
@@ -2269,7 +2278,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -2296,7 +2305,7 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B63" t="s">
         <v>24</v>
@@ -2323,7 +2332,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>24</v>
@@ -2350,7 +2359,7 @@
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>24</v>
@@ -2377,7 +2386,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>24</v>
@@ -2404,10 +2413,10 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C67" t="s">
         <v>18</v>
@@ -2431,7 +2440,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -2458,7 +2467,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>20</v>
@@ -2485,7 +2494,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
         <v>24</v>
@@ -2512,7 +2521,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B71" t="s">
         <v>24</v>
@@ -2539,7 +2548,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B72" t="s">
         <v>24</v>
@@ -2566,7 +2575,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B73" t="s">
         <v>24</v>
@@ -2593,7 +2602,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
@@ -2620,7 +2629,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
@@ -2647,7 +2656,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B76" t="s">
         <v>10</v>
@@ -2674,7 +2683,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B77" t="s">
         <v>24</v>
@@ -2701,7 +2710,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B78" t="s">
         <v>24</v>
@@ -2728,7 +2737,7 @@
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B79" t="s">
         <v>24</v>
@@ -2755,7 +2764,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
         <v>10</v>
@@ -2782,7 +2791,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
@@ -2809,7 +2818,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B82" t="s">
         <v>20</v>
@@ -2836,7 +2845,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B83" t="s">
         <v>24</v>
@@ -2863,7 +2872,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B84" t="s">
         <v>24</v>
@@ -2890,7 +2899,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="B85" t="s">
         <v>24</v>
@@ -2917,10 +2926,10 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B86" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C86" t="s">
         <v>18</v>
@@ -2944,7 +2953,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
@@ -2971,61 +2980,61 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B88" t="s">
         <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D88" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E88">
-        <v>2792</v>
+        <v>2761</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
       </c>
       <c r="G88" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H88" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="I88"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B89" t="s">
         <v>24</v>
       </c>
       <c r="C89" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D89" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E89">
-        <v>2761</v>
+        <v>2792</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="H89" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="I89"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B90" t="s">
         <v>24</v>
@@ -3052,7 +3061,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B91" t="s">
         <v>24</v>
@@ -3079,7 +3088,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B92" t="s">
         <v>10</v>
@@ -3106,7 +3115,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B93" t="s">
         <v>10</v>
@@ -3133,7 +3142,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B94" t="s">
         <v>20</v>
@@ -3160,7 +3169,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B95" t="s">
         <v>24</v>
@@ -3187,7 +3196,7 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B96" t="s">
         <v>24</v>
@@ -3214,10 +3223,10 @@
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="B97" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C97" t="s">
         <v>29</v>
@@ -3241,7 +3250,7 @@
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B98" t="s">
         <v>20</v>
@@ -3268,7 +3277,7 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B99" t="s">
         <v>24</v>
@@ -3295,7 +3304,7 @@
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B100" t="s">
         <v>20</v>
@@ -3322,7 +3331,7 @@
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B101" t="s">
         <v>20</v>
@@ -3349,7 +3358,7 @@
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B102" t="s">
         <v>20</v>
@@ -3376,7 +3385,7 @@
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B103" t="s">
         <v>24</v>
@@ -3403,7 +3412,7 @@
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B104" t="s">
         <v>10</v>
@@ -3430,7 +3439,7 @@
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
@@ -3457,7 +3466,7 @@
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B106" t="s">
         <v>20</v>
@@ -3484,25 +3493,25 @@
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B107" t="s">
         <v>24</v>
       </c>
       <c r="C107" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E107">
-        <v>3332</v>
+        <v>3271</v>
       </c>
       <c r="F107" t="s">
         <v>13</v>
       </c>
       <c r="G107" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="H107" t="s">
         <v>15</v>
@@ -3511,25 +3520,25 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B108" t="s">
         <v>24</v>
       </c>
       <c r="C108" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D108" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E108">
-        <v>3271</v>
+        <v>3332</v>
       </c>
       <c r="F108" t="s">
         <v>13</v>
       </c>
       <c r="G108" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="H108" t="s">
         <v>15</v>
@@ -3538,10 +3547,10 @@
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B109" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C109" t="s">
         <v>18</v>
@@ -3565,10 +3574,10 @@
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B110" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C110" t="s">
         <v>33</v>
@@ -3592,7 +3601,7 @@
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
@@ -3619,7 +3628,7 @@
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B112" t="s">
         <v>24</v>
@@ -3646,7 +3655,7 @@
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B113" t="s">
         <v>24</v>
@@ -3673,7 +3682,7 @@
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B114" t="s">
         <v>24</v>
@@ -3700,7 +3709,7 @@
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B115" t="s">
         <v>24</v>
@@ -3727,7 +3736,7 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B116" t="s">
         <v>10</v>
@@ -3754,7 +3763,7 @@
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B117" t="s">
         <v>10</v>
@@ -3781,7 +3790,7 @@
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B118" t="s">
         <v>24</v>
@@ -3808,7 +3817,7 @@
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B119" t="s">
         <v>24</v>
@@ -3835,7 +3844,7 @@
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B120" t="s">
         <v>24</v>
@@ -3862,10 +3871,10 @@
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B121" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C121" t="s">
         <v>12</v>
@@ -3889,7 +3898,7 @@
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B122" t="s">
         <v>20</v>
@@ -3916,7 +3925,7 @@
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B123" t="s">
         <v>20</v>
@@ -3943,7 +3952,7 @@
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B124" t="s">
         <v>20</v>
@@ -3970,7 +3979,7 @@
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B125" t="s">
         <v>20</v>
@@ -3997,7 +4006,7 @@
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B126" t="s">
         <v>20</v>
@@ -4024,7 +4033,7 @@
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="B127" t="s">
         <v>20</v>
@@ -4051,7 +4060,7 @@
     </row>
     <row r="128" spans="1:9">
       <c r="A128" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B128" t="s">
         <v>20</v>
@@ -4078,7 +4087,7 @@
     </row>
     <row r="129" spans="1:9">
       <c r="A129" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B129" t="s">
         <v>20</v>
@@ -4105,7 +4114,7 @@
     </row>
     <row r="130" spans="1:9">
       <c r="A130" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B130" t="s">
         <v>20</v>
@@ -4132,7 +4141,7 @@
     </row>
     <row r="131" spans="1:9">
       <c r="A131" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B131" t="s">
         <v>20</v>
@@ -4159,7 +4168,7 @@
     </row>
     <row r="132" spans="1:9">
       <c r="A132" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B132" t="s">
         <v>20</v>
@@ -4186,7 +4195,7 @@
     </row>
     <row r="133" spans="1:9">
       <c r="A133" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B133" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
fix: lookup team for handbal nl
</commit_message>
<xml_diff>
--- a/static/handbalnl/programma.xlsx
+++ b/static/handbalnl/programma.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="81">
   <si>
     <t>Datum</t>
   </si>
@@ -44,166 +44,154 @@
     <t>Uitslagen</t>
   </si>
   <si>
-    <t>07-09-2024</t>
+    <t>14-09-2024</t>
   </si>
   <si>
     <t>19:00:00</t>
   </si>
   <si>
+    <t>KRAS/Volendam HS1</t>
+  </si>
+  <si>
+    <t>JD Techniek/ Hurry-up HS1</t>
+  </si>
+  <si>
+    <t>Heren Super Handball League Super Handball League</t>
+  </si>
+  <si>
+    <t>Sporthal Opperdam</t>
+  </si>
+  <si>
+    <t>zaal 2 (oud)</t>
+  </si>
+  <si>
+    <t>20:00:00</t>
+  </si>
+  <si>
+    <t>LIMBURG LIONS/ Sittardia HS1</t>
+  </si>
+  <si>
+    <t>HUBO Handbal HS1</t>
+  </si>
+  <si>
+    <t>Stadssporthal</t>
+  </si>
+  <si>
+    <t>zaal 1</t>
+  </si>
+  <si>
+    <t>20:15:00</t>
+  </si>
+  <si>
+    <t>KTSV Eupen HS1</t>
+  </si>
+  <si>
+    <t>Green Park/Handbal Aalsmeer HS1</t>
+  </si>
+  <si>
+    <t>Sporthalle Stockbergerweg</t>
+  </si>
+  <si>
+    <t>zaal</t>
+  </si>
+  <si>
+    <t>Sezoens Achilles Bocholt HS1</t>
+  </si>
+  <si>
+    <t>Herpertz/Bevo HC HS1</t>
+  </si>
+  <si>
+    <t>De Damburg (B)</t>
+  </si>
+  <si>
+    <t>Biobest/ Sasja HC HS1</t>
+  </si>
+  <si>
     <t>LvanRaak Milieu/Handbal Houten HS1</t>
   </si>
   <si>
-    <t>KRAS/Volendam HS1</t>
-  </si>
-  <si>
-    <t>Heren Super Handball League Super Handball League</t>
+    <t>Sorghvliedt Sporthal (B)</t>
+  </si>
+  <si>
+    <t>HC Visé BM HS1</t>
+  </si>
+  <si>
+    <t>Sporting Pelt HS1</t>
+  </si>
+  <si>
+    <t>Hall Omnisport De Visé (B)</t>
+  </si>
+  <si>
+    <t>21-09-2024</t>
+  </si>
+  <si>
+    <t>Sporthal de Bloemhof</t>
+  </si>
+  <si>
+    <t>De Eendracht</t>
+  </si>
+  <si>
+    <t>De Heuf</t>
+  </si>
+  <si>
+    <t>Dommelhof (B)</t>
+  </si>
+  <si>
+    <t>Alverberg (B)</t>
+  </si>
+  <si>
+    <t>28-09-2024</t>
   </si>
   <si>
     <t>Sporthal The Dome</t>
   </si>
   <si>
-    <t>zaal 1</t>
-  </si>
-  <si>
-    <t>19:30:00</t>
-  </si>
-  <si>
-    <t>Green Park/Handbal Aalsmeer HS1</t>
-  </si>
-  <si>
-    <t>Biobest/ Sasja HC HS1</t>
-  </si>
-  <si>
-    <t>Sporthal de Bloemhof</t>
-  </si>
-  <si>
-    <t>20:00:00</t>
-  </si>
-  <si>
-    <t>JD Techniek/ Hurry-up HS1</t>
-  </si>
-  <si>
-    <t>HC Visé BM HS1</t>
-  </si>
-  <si>
-    <t>De Eendracht</t>
-  </si>
-  <si>
-    <t>20:15:00</t>
-  </si>
-  <si>
-    <t>Herpertz/Bevo HC HS1</t>
-  </si>
-  <si>
-    <t>KEMBIT-LIONS/Sittardia HS1</t>
-  </si>
-  <si>
-    <t>De Heuf</t>
-  </si>
-  <si>
-    <t>Sporting Pelt HS1</t>
-  </si>
-  <si>
-    <t>Sezoens Achilles Bocholt HS1</t>
-  </si>
-  <si>
-    <t>Dommelhof (B)</t>
-  </si>
-  <si>
-    <t>08-09-2024</t>
-  </si>
-  <si>
-    <t>16:15:00</t>
-  </si>
-  <si>
-    <t>HUBO Handbal HS1</t>
-  </si>
-  <si>
-    <t>KTSV Eupen (B) HS1</t>
+    <t>29-09-2024</t>
+  </si>
+  <si>
+    <t>14:00:00</t>
+  </si>
+  <si>
+    <t>05-10-2024</t>
+  </si>
+  <si>
+    <t>06-10-2024</t>
+  </si>
+  <si>
+    <t>15:10:00</t>
+  </si>
+  <si>
+    <t>12-10-2024</t>
+  </si>
+  <si>
+    <t>15-10-2024</t>
+  </si>
+  <si>
+    <t>20:30:00</t>
+  </si>
+  <si>
+    <t>16-10-2024</t>
+  </si>
+  <si>
+    <t>19-10-2024</t>
+  </si>
+  <si>
+    <t>22-10-2024</t>
+  </si>
+  <si>
+    <t>26-10-2024</t>
+  </si>
+  <si>
+    <t>02-11-2024</t>
+  </si>
+  <si>
+    <t>03-11-2024</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Eburons Dôme </t>
-  </si>
-  <si>
-    <t>14-09-2024</t>
-  </si>
-  <si>
-    <t>Sporthal Opperdam</t>
-  </si>
-  <si>
-    <t>zaal 2 (oud)</t>
-  </si>
-  <si>
-    <t>Stadssporthal</t>
-  </si>
-  <si>
-    <t>Sporthalle Stockbergerweg</t>
-  </si>
-  <si>
-    <t>zaal</t>
-  </si>
-  <si>
-    <t>De Damburg (B)</t>
-  </si>
-  <si>
-    <t>Sorghvliedt Sporthal (B)</t>
-  </si>
-  <si>
-    <t>Hall Omnisport De Visé (B)</t>
-  </si>
-  <si>
-    <t>21-09-2024</t>
-  </si>
-  <si>
-    <t>Alverberg (B)</t>
-  </si>
-  <si>
-    <t>28-09-2024</t>
-  </si>
-  <si>
-    <t>29-09-2024</t>
-  </si>
-  <si>
-    <t>14:00:00</t>
-  </si>
-  <si>
-    <t>05-10-2024</t>
-  </si>
-  <si>
-    <t>06-10-2024</t>
-  </si>
-  <si>
-    <t>15:10:00</t>
-  </si>
-  <si>
-    <t>12-10-2024</t>
-  </si>
-  <si>
-    <t>15-10-2024</t>
-  </si>
-  <si>
-    <t>20:30:00</t>
-  </si>
-  <si>
-    <t>16-10-2024</t>
-  </si>
-  <si>
-    <t>19-10-2024</t>
-  </si>
-  <si>
-    <t>22-10-2024</t>
-  </si>
-  <si>
-    <t>26-10-2024</t>
-  </si>
-  <si>
-    <t>02-11-2024</t>
-  </si>
-  <si>
-    <t>03-11-2024</t>
-  </si>
-  <si>
-    <t>15:00:00</t>
   </si>
   <si>
     <t>16-11-2024</t>
@@ -608,7 +596,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -670,7 +658,7 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>313</v>
+        <v>493</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -697,7 +685,7 @@
         <v>18</v>
       </c>
       <c r="E3">
-        <v>163</v>
+        <v>403</v>
       </c>
       <c r="F3" t="s">
         <v>13</v>
@@ -706,7 +694,7 @@
         <v>19</v>
       </c>
       <c r="H3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I3"/>
     </row>
@@ -715,25 +703,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4">
-        <v>283</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I4"/>
     </row>
@@ -742,25 +730,25 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5">
-        <v>224</v>
+        <v>434</v>
       </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I5"/>
     </row>
@@ -769,220 +757,220 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <v>252</v>
+        <v>343</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I6"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>33</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7">
+        <v>463</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>34</v>
       </c>
-      <c r="E7">
-        <v>193</v>
-      </c>
-      <c r="F7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
       <c r="H7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I7"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E8">
-        <v>493</v>
+        <v>524</v>
       </c>
       <c r="F8" t="s">
         <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I8"/>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E9">
-        <v>403</v>
+        <v>675</v>
       </c>
       <c r="F9" t="s">
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H9" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I9"/>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="E10">
-        <v>373</v>
+        <v>616</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I10"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>584</v>
+      </c>
+      <c r="F11" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="H11" t="s">
         <v>25</v>
-      </c>
-      <c r="E11">
-        <v>434</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" t="s">
-        <v>15</v>
       </c>
       <c r="I11"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
       </c>
       <c r="E12">
-        <v>343</v>
+        <v>645</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I12"/>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E13">
-        <v>463</v>
+        <v>554</v>
       </c>
       <c r="F13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I13"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
@@ -991,10 +979,10 @@
         <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E14">
-        <v>524</v>
+        <v>734</v>
       </c>
       <c r="F14" t="s">
         <v>13</v>
@@ -1003,139 +991,139 @@
         <v>19</v>
       </c>
       <c r="H14" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I14"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="E15">
-        <v>675</v>
+        <v>824</v>
       </c>
       <c r="F15" t="s">
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="H15" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I15"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E16">
-        <v>616</v>
+        <v>2850</v>
       </c>
       <c r="F16" t="s">
         <v>13</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I16"/>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E17">
-        <v>584</v>
+        <v>765</v>
       </c>
       <c r="F17" t="s">
         <v>13</v>
       </c>
       <c r="G17" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="H17" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I17"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E18">
-        <v>645</v>
+        <v>796</v>
       </c>
       <c r="F18" t="s">
         <v>13</v>
       </c>
       <c r="G18" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I18"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E19">
-        <v>554</v>
+        <v>855</v>
       </c>
       <c r="F19" t="s">
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
         <v>15</v>
@@ -1144,187 +1132,187 @@
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E20">
-        <v>734</v>
+        <v>1007</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
       </c>
       <c r="G20" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="H20" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I20"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E21">
-        <v>824</v>
+        <v>946</v>
       </c>
       <c r="F21" t="s">
         <v>13</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H21" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I21"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="E22">
-        <v>2850</v>
+        <v>977</v>
       </c>
       <c r="F22" t="s">
         <v>13</v>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="H22" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I22"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E23">
-        <v>765</v>
+        <v>1036</v>
       </c>
       <c r="F23" t="s">
         <v>13</v>
       </c>
       <c r="G23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I23"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E24">
-        <v>796</v>
+        <v>917</v>
       </c>
       <c r="F24" t="s">
         <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I24"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E25">
-        <v>855</v>
+        <v>887</v>
       </c>
       <c r="F25" t="s">
         <v>13</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H25" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I25"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B26" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E26">
-        <v>1007</v>
+        <v>1217</v>
       </c>
       <c r="F26" t="s">
         <v>13</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H26" t="s">
         <v>15</v>
@@ -1333,349 +1321,349 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D27" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="E27">
-        <v>946</v>
+        <v>1186</v>
       </c>
       <c r="F27" t="s">
         <v>13</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I27"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="E28">
-        <v>977</v>
+        <v>1126</v>
       </c>
       <c r="F28" t="s">
         <v>13</v>
       </c>
       <c r="G28" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="H28" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I28"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E29">
-        <v>1036</v>
+        <v>1065</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
       </c>
       <c r="G29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H29" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I29"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D30" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="E30">
-        <v>917</v>
+        <v>1095</v>
       </c>
       <c r="F30" t="s">
         <v>13</v>
       </c>
       <c r="G30" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I30"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
         <v>22</v>
       </c>
       <c r="E31">
-        <v>887</v>
+        <v>1156</v>
       </c>
       <c r="F31" t="s">
         <v>13</v>
       </c>
       <c r="G31" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I31"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E32">
-        <v>1217</v>
+        <v>1397</v>
       </c>
       <c r="F32" t="s">
         <v>13</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="H32" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I32"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C33" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D33" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E33">
-        <v>1186</v>
+        <v>1278</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
       </c>
       <c r="G33" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="H33" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I33"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D34" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E34">
-        <v>1126</v>
+        <v>1248</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="H34" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I34"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B35" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E35">
-        <v>1095</v>
+        <v>1367</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>
       </c>
       <c r="G35" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I35"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36">
+        <v>1307</v>
+      </c>
+      <c r="F36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G36" t="s">
         <v>24</v>
       </c>
-      <c r="C36" t="s">
-        <v>18</v>
-      </c>
-      <c r="D36" t="s">
-        <v>28</v>
-      </c>
-      <c r="E36">
-        <v>1065</v>
-      </c>
-      <c r="F36" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" t="s">
-        <v>43</v>
-      </c>
       <c r="H36" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I36"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E37">
-        <v>1156</v>
+        <v>1336</v>
       </c>
       <c r="F37" t="s">
         <v>13</v>
       </c>
       <c r="G37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H37" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I37"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E38">
-        <v>1397</v>
+        <v>1488</v>
       </c>
       <c r="F38" t="s">
         <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="H38" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I38"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E39">
-        <v>1278</v>
+        <v>1579</v>
       </c>
       <c r="F39" t="s">
         <v>13</v>
       </c>
       <c r="G39" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="H39" t="s">
         <v>15</v>
@@ -1684,295 +1672,295 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B40" t="s">
         <v>10</v>
       </c>
       <c r="C40" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E40">
-        <v>1248</v>
+        <v>1548</v>
       </c>
       <c r="F40" t="s">
         <v>13</v>
       </c>
       <c r="G40" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H40" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I40"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E41">
-        <v>1367</v>
+        <v>1428</v>
       </c>
       <c r="F41" t="s">
         <v>13</v>
       </c>
       <c r="G41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H41" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I41"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E42">
-        <v>1307</v>
+        <v>1456</v>
       </c>
       <c r="F42" t="s">
         <v>13</v>
       </c>
       <c r="G42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H42" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I42"/>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C43" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D43" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E43">
-        <v>1336</v>
+        <v>1519</v>
       </c>
       <c r="F43" t="s">
         <v>13</v>
       </c>
       <c r="G43" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H43" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I43"/>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B44" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D44" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="E44">
-        <v>1488</v>
+        <v>1609</v>
       </c>
       <c r="F44" t="s">
         <v>13</v>
       </c>
       <c r="G44" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="H44" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I44"/>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C45" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" t="s">
         <v>12</v>
       </c>
-      <c r="D45" t="s">
-        <v>26</v>
-      </c>
       <c r="E45">
-        <v>1579</v>
+        <v>1701</v>
       </c>
       <c r="F45" t="s">
         <v>13</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="H45" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="I45"/>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B46" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C46" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D46" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E46">
-        <v>1548</v>
+        <v>1732</v>
       </c>
       <c r="F46" t="s">
         <v>13</v>
       </c>
       <c r="G46" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H46" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I46"/>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B47" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D47" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E47">
-        <v>1428</v>
+        <v>1762</v>
       </c>
       <c r="F47" t="s">
         <v>13</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H47" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I47"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B48" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D48" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E48">
-        <v>1456</v>
+        <v>3696</v>
       </c>
       <c r="F48" t="s">
         <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H48" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I48"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B49" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D49" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E49">
-        <v>1519</v>
+        <v>1671</v>
       </c>
       <c r="F49" t="s">
         <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="H49" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I49"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
         <v>10</v>
       </c>
       <c r="C50" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D50" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E50">
-        <v>1609</v>
+        <v>1946</v>
       </c>
       <c r="F50" t="s">
         <v>13</v>
       </c>
       <c r="G50" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H50" t="s">
         <v>15</v>
@@ -1981,322 +1969,322 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C51" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D51" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E51">
-        <v>1701</v>
+        <v>1914</v>
       </c>
       <c r="F51" t="s">
         <v>13</v>
       </c>
       <c r="G51" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H51" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I51"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B52" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C52" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E52">
-        <v>1732</v>
+        <v>1883</v>
       </c>
       <c r="F52" t="s">
         <v>13</v>
       </c>
       <c r="G52" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H52" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I52"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C53" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D53" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E53">
-        <v>1762</v>
+        <v>1825</v>
       </c>
       <c r="F53" t="s">
         <v>13</v>
       </c>
       <c r="G53" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="H53" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I53"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B54" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C54" t="s">
+        <v>33</v>
+      </c>
+      <c r="D54" t="s">
         <v>22</v>
       </c>
-      <c r="D54" t="s">
-        <v>18</v>
-      </c>
       <c r="E54">
-        <v>3696</v>
+        <v>1853</v>
       </c>
       <c r="F54" t="s">
         <v>13</v>
       </c>
       <c r="G54" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H54" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I54"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>21</v>
       </c>
       <c r="C55" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D55" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E55">
-        <v>1671</v>
+        <v>1793</v>
       </c>
       <c r="F55" t="s">
         <v>13</v>
       </c>
       <c r="G55" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="H55" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I55"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B56" t="s">
         <v>10</v>
       </c>
       <c r="C56" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D56" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E56">
-        <v>1946</v>
+        <v>1977</v>
       </c>
       <c r="F56" t="s">
         <v>13</v>
       </c>
       <c r="G56" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H56" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I56"/>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B57" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C57" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D57" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E57">
-        <v>1914</v>
+        <v>2037</v>
       </c>
       <c r="F57" t="s">
         <v>13</v>
       </c>
       <c r="G57" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H57" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I57"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D58" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E58">
-        <v>1883</v>
+        <v>2066</v>
       </c>
       <c r="F58" t="s">
         <v>13</v>
       </c>
       <c r="G58" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="H58" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I58"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B59" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C59" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D59" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E59">
-        <v>1825</v>
+        <v>2096</v>
       </c>
       <c r="F59" t="s">
         <v>13</v>
       </c>
       <c r="G59" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H59" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I59"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D60" t="s">
+        <v>30</v>
+      </c>
+      <c r="E60">
+        <v>2127</v>
+      </c>
+      <c r="F60" t="s">
+        <v>13</v>
+      </c>
+      <c r="G60" t="s">
         <v>34</v>
       </c>
-      <c r="E60">
-        <v>1853</v>
-      </c>
-      <c r="F60" t="s">
-        <v>13</v>
-      </c>
-      <c r="G60" t="s">
-        <v>30</v>
-      </c>
       <c r="H60" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I60"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C61" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D61" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E61">
-        <v>1793</v>
+        <v>2007</v>
       </c>
       <c r="F61" t="s">
         <v>13</v>
       </c>
       <c r="G61" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H61" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I61"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
       </c>
       <c r="C62" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E62">
-        <v>1977</v>
+        <v>2308</v>
       </c>
       <c r="F62" t="s">
         <v>13</v>
       </c>
       <c r="G62" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H62" t="s">
         <v>15</v>
@@ -2305,142 +2293,142 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C63" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D63" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E63">
-        <v>2037</v>
+        <v>2219</v>
       </c>
       <c r="F63" t="s">
         <v>13</v>
       </c>
       <c r="G63" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="H63" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I63"/>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" t="s">
+        <v>22</v>
+      </c>
+      <c r="D64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64">
+        <v>2188</v>
+      </c>
+      <c r="F64" t="s">
+        <v>13</v>
+      </c>
+      <c r="G64" t="s">
         <v>24</v>
       </c>
-      <c r="C64" t="s">
-        <v>26</v>
-      </c>
-      <c r="D64" t="s">
-        <v>28</v>
-      </c>
-      <c r="E64">
-        <v>2066</v>
-      </c>
-      <c r="F64" t="s">
-        <v>13</v>
-      </c>
-      <c r="G64" t="s">
-        <v>39</v>
-      </c>
       <c r="H64" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I64"/>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E65">
-        <v>2096</v>
+        <v>2247</v>
       </c>
       <c r="F65" t="s">
         <v>13</v>
       </c>
       <c r="G65" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H65" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I65"/>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C66" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E66">
-        <v>2127</v>
+        <v>2158</v>
       </c>
       <c r="F66" t="s">
         <v>13</v>
       </c>
       <c r="G66" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="H66" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I66"/>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="C67" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D67" t="s">
         <v>12</v>
       </c>
       <c r="E67">
-        <v>2007</v>
+        <v>2278</v>
       </c>
       <c r="F67" t="s">
         <v>13</v>
       </c>
       <c r="G67" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H67" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I67"/>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B68" t="s">
         <v>10</v>
@@ -2452,7 +2440,7 @@
         <v>11</v>
       </c>
       <c r="E68">
-        <v>2308</v>
+        <v>2458</v>
       </c>
       <c r="F68" t="s">
         <v>13</v>
@@ -2461,166 +2449,166 @@
         <v>37</v>
       </c>
       <c r="H68" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I68"/>
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B69" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C69" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D69" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E69">
-        <v>2219</v>
+        <v>2338</v>
       </c>
       <c r="F69" t="s">
         <v>13</v>
       </c>
       <c r="G69" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H69" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I69"/>
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B70" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C70" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D70" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E70">
-        <v>2188</v>
+        <v>2488</v>
       </c>
       <c r="F70" t="s">
         <v>13</v>
       </c>
       <c r="G70" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H70" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I70"/>
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B71" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C71" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="E71">
-        <v>2158</v>
+        <v>2399</v>
       </c>
       <c r="F71" t="s">
         <v>13</v>
       </c>
       <c r="G71" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="H71" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I71"/>
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B72" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D72" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E72">
-        <v>2247</v>
+        <v>2428</v>
       </c>
       <c r="F72" t="s">
         <v>13</v>
       </c>
       <c r="G72" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H72" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I72"/>
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B73" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C73" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D73" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E73">
-        <v>2278</v>
+        <v>2368</v>
       </c>
       <c r="F73" t="s">
         <v>13</v>
       </c>
       <c r="G73" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H73" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I73"/>
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B74" t="s">
         <v>10</v>
       </c>
       <c r="C74" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D74" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
       <c r="E74">
-        <v>2458</v>
+        <v>2670</v>
       </c>
       <c r="F74" t="s">
         <v>13</v>
       </c>
       <c r="G74" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H74" t="s">
         <v>15</v>
@@ -2629,322 +2617,322 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B75" t="s">
         <v>10</v>
       </c>
       <c r="C75" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D75" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="E75">
-        <v>2338</v>
+        <v>2641</v>
       </c>
       <c r="F75" t="s">
         <v>13</v>
       </c>
       <c r="G75" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H75" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I75"/>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D76" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E76">
-        <v>2488</v>
+        <v>2549</v>
       </c>
       <c r="F76" t="s">
         <v>13</v>
       </c>
       <c r="G76" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H76" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I76"/>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B77" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C77" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D77" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E77">
-        <v>2399</v>
+        <v>2611</v>
       </c>
       <c r="F77" t="s">
         <v>13</v>
       </c>
       <c r="G77" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H77" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I77"/>
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B78" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78">
+        <v>2579</v>
+      </c>
+      <c r="F78" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" t="s">
         <v>28</v>
       </c>
-      <c r="D78" t="s">
-        <v>22</v>
-      </c>
-      <c r="E78">
-        <v>2428</v>
-      </c>
-      <c r="F78" t="s">
-        <v>13</v>
-      </c>
-      <c r="G78" t="s">
-        <v>30</v>
-      </c>
       <c r="H78" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I78"/>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B79" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C79" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D79" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E79">
-        <v>2368</v>
+        <v>2518</v>
       </c>
       <c r="F79" t="s">
         <v>13</v>
       </c>
       <c r="G79" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H79" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I79"/>
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="C80" t="s">
+        <v>29</v>
+      </c>
+      <c r="D80" t="s">
         <v>12</v>
       </c>
-      <c r="D80" t="s">
-        <v>28</v>
-      </c>
       <c r="E80">
-        <v>2670</v>
+        <v>705</v>
       </c>
       <c r="F80" t="s">
         <v>13</v>
       </c>
       <c r="G80" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H80" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I80"/>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B81" t="s">
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D81" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E81">
-        <v>2641</v>
+        <v>2701</v>
       </c>
       <c r="F81" t="s">
         <v>13</v>
       </c>
       <c r="G81" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="H81" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I81"/>
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B82" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C82" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D82" t="s">
         <v>17</v>
       </c>
       <c r="E82">
-        <v>2549</v>
+        <v>2761</v>
       </c>
       <c r="F82" t="s">
         <v>13</v>
       </c>
       <c r="G82" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="H82" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I82"/>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B83" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C83" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D83" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E83">
-        <v>2611</v>
+        <v>2792</v>
       </c>
       <c r="F83" t="s">
         <v>13</v>
       </c>
       <c r="G83" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H83" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I83"/>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B84" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D84" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E84">
-        <v>2579</v>
+        <v>2820</v>
       </c>
       <c r="F84" t="s">
         <v>13</v>
       </c>
       <c r="G84" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H84" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I84"/>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B85" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C85" t="s">
         <v>18</v>
       </c>
       <c r="D85" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E85">
-        <v>2518</v>
+        <v>2732</v>
       </c>
       <c r="F85" t="s">
         <v>13</v>
       </c>
       <c r="G85" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="H85" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I85"/>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B86" t="s">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C86" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" t="s">
         <v>18</v>
       </c>
-      <c r="D86" t="s">
-        <v>21</v>
-      </c>
       <c r="E86">
-        <v>705</v>
+        <v>3031</v>
       </c>
       <c r="F86" t="s">
         <v>13</v>
       </c>
       <c r="G86" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="H86" t="s">
         <v>15</v>
@@ -2953,190 +2941,190 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B87" t="s">
         <v>10</v>
       </c>
       <c r="C87" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D87" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E87">
-        <v>2701</v>
+        <v>3001</v>
       </c>
       <c r="F87" t="s">
         <v>13</v>
       </c>
       <c r="G87" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H87" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I87"/>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B88" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C88" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D88" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E88">
-        <v>2761</v>
+        <v>2938</v>
       </c>
       <c r="F88" t="s">
         <v>13</v>
       </c>
       <c r="G88" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H88" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I88"/>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B89" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D89" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E89">
-        <v>2792</v>
+        <v>2970</v>
       </c>
       <c r="F89" t="s">
         <v>13</v>
       </c>
       <c r="G89" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="H89" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I89"/>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B90" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C90" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E90">
-        <v>2820</v>
+        <v>2880</v>
       </c>
       <c r="F90" t="s">
         <v>13</v>
       </c>
       <c r="G90" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H90" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I90"/>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
+        <v>69</v>
+      </c>
+      <c r="B91" t="s">
         <v>70</v>
       </c>
-      <c r="B91" t="s">
-        <v>24</v>
-      </c>
       <c r="C91" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D91" t="s">
         <v>22</v>
       </c>
       <c r="E91">
-        <v>2732</v>
+        <v>2909</v>
       </c>
       <c r="F91" t="s">
         <v>13</v>
       </c>
       <c r="G91" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H91" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I91"/>
     </row>
     <row r="92" spans="1:9">
       <c r="A92" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B92" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D92" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="E92">
-        <v>3031</v>
+        <v>3062</v>
       </c>
       <c r="F92" t="s">
         <v>13</v>
       </c>
       <c r="G92" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H92" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I92"/>
     </row>
     <row r="93" spans="1:9">
       <c r="A93" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B93" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C93" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D93" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E93">
-        <v>3001</v>
+        <v>3092</v>
       </c>
       <c r="F93" t="s">
         <v>13</v>
       </c>
       <c r="G93" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="H93" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I93"/>
     </row>
@@ -3145,25 +3133,25 @@
         <v>72</v>
       </c>
       <c r="B94" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C94" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D94" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E94">
-        <v>2938</v>
+        <v>3122</v>
       </c>
       <c r="F94" t="s">
         <v>13</v>
       </c>
       <c r="G94" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H94" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I94"/>
     </row>
@@ -3172,25 +3160,25 @@
         <v>72</v>
       </c>
       <c r="B95" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C95" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E95">
-        <v>2970</v>
+        <v>3153</v>
       </c>
       <c r="F95" t="s">
         <v>13</v>
       </c>
       <c r="G95" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="H95" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I95"/>
     </row>
@@ -3199,76 +3187,76 @@
         <v>72</v>
       </c>
       <c r="B96" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C96" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D96" t="s">
         <v>26</v>
       </c>
       <c r="E96">
-        <v>2880</v>
+        <v>3183</v>
       </c>
       <c r="F96" t="s">
         <v>13</v>
       </c>
       <c r="G96" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="H96" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I96"/>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="C97" t="s">
+        <v>33</v>
+      </c>
+      <c r="D97" t="s">
         <v>29</v>
       </c>
-      <c r="D97" t="s">
-        <v>34</v>
-      </c>
       <c r="E97">
-        <v>2909</v>
+        <v>3212</v>
       </c>
       <c r="F97" t="s">
         <v>13</v>
       </c>
       <c r="G97" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H97" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I97"/>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B98" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D98" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="E98">
-        <v>3062</v>
+        <v>3392</v>
       </c>
       <c r="F98" t="s">
         <v>13</v>
       </c>
       <c r="G98" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H98" t="s">
         <v>15</v>
@@ -3277,457 +3265,457 @@
     </row>
     <row r="99" spans="1:9">
       <c r="A99" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B99" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C99" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D99" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="E99">
-        <v>3092</v>
+        <v>3363</v>
       </c>
       <c r="F99" t="s">
         <v>13</v>
       </c>
       <c r="G99" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="H99" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I99"/>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B100" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C100" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D100" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E100">
-        <v>3122</v>
+        <v>3301</v>
       </c>
       <c r="F100" t="s">
         <v>13</v>
       </c>
       <c r="G100" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H100" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I100"/>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B101" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C101" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E101">
-        <v>3153</v>
+        <v>3271</v>
       </c>
       <c r="F101" t="s">
         <v>13</v>
       </c>
       <c r="G101" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H101" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I101"/>
     </row>
     <row r="102" spans="1:9">
       <c r="A102" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B102" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C102" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D102" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="E102">
-        <v>3183</v>
+        <v>3332</v>
       </c>
       <c r="F102" t="s">
         <v>13</v>
       </c>
       <c r="G102" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H102" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I102"/>
     </row>
     <row r="103" spans="1:9">
       <c r="A103" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B103" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C103" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D103" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="E103">
-        <v>3212</v>
+        <v>3242</v>
       </c>
       <c r="F103" t="s">
         <v>13</v>
       </c>
       <c r="G103" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H103" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I103"/>
     </row>
     <row r="104" spans="1:9">
       <c r="A104" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B104" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="C104" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D104" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E104">
-        <v>3392</v>
+        <v>3483</v>
       </c>
       <c r="F104" t="s">
         <v>13</v>
       </c>
       <c r="G104" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="H104" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I104"/>
     </row>
     <row r="105" spans="1:9">
       <c r="A105" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B105" t="s">
         <v>10</v>
       </c>
       <c r="C105" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D105" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="E105">
-        <v>3363</v>
+        <v>3424</v>
       </c>
       <c r="F105" t="s">
         <v>13</v>
       </c>
       <c r="G105" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="H105" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I105"/>
     </row>
     <row r="106" spans="1:9">
       <c r="A106" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B106" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C106" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D106" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E106">
-        <v>3301</v>
+        <v>3512</v>
       </c>
       <c r="F106" t="s">
         <v>13</v>
       </c>
       <c r="G106" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H106" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I106"/>
     </row>
     <row r="107" spans="1:9">
       <c r="A107" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B107" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C107" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D107" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E107">
-        <v>3271</v>
+        <v>3543</v>
       </c>
       <c r="F107" t="s">
         <v>13</v>
       </c>
       <c r="G107" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="H107" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I107"/>
     </row>
     <row r="108" spans="1:9">
       <c r="A108" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B108" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C108" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D108" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E108">
-        <v>3332</v>
+        <v>3455</v>
       </c>
       <c r="F108" t="s">
         <v>13</v>
       </c>
       <c r="G108" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="H108" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I108"/>
     </row>
     <row r="109" spans="1:9">
       <c r="A109" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="C109" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="D109" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E109">
-        <v>3242</v>
+        <v>3574</v>
       </c>
       <c r="F109" t="s">
         <v>13</v>
       </c>
       <c r="G109" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="H109" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I109"/>
     </row>
     <row r="110" spans="1:9">
       <c r="A110" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B110" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C110" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D110" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E110">
-        <v>3483</v>
+        <v>3665</v>
       </c>
       <c r="F110" t="s">
         <v>13</v>
       </c>
       <c r="G110" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H110" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I110"/>
     </row>
     <row r="111" spans="1:9">
       <c r="A111" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B111" t="s">
         <v>10</v>
       </c>
       <c r="C111" t="s">
+        <v>30</v>
+      </c>
+      <c r="D111" t="s">
         <v>17</v>
       </c>
-      <c r="D111" t="s">
-        <v>21</v>
-      </c>
       <c r="E111">
-        <v>3424</v>
+        <v>3727</v>
       </c>
       <c r="F111" t="s">
         <v>13</v>
       </c>
       <c r="G111" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="H111" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I111"/>
     </row>
     <row r="112" spans="1:9">
       <c r="A112" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C112" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D112" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E112">
-        <v>3512</v>
+        <v>1640</v>
       </c>
       <c r="F112" t="s">
         <v>13</v>
       </c>
       <c r="G112" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="H112" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I112"/>
     </row>
     <row r="113" spans="1:9">
       <c r="A113" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C113" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D113" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E113">
-        <v>3543</v>
+        <v>3605</v>
       </c>
       <c r="F113" t="s">
         <v>13</v>
       </c>
       <c r="G113" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H113" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I113"/>
     </row>
     <row r="114" spans="1:9">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C114" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D114" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E114">
-        <v>3455</v>
+        <v>3635</v>
       </c>
       <c r="F114" t="s">
         <v>13</v>
       </c>
       <c r="G114" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H114" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I114"/>
     </row>
     <row r="115" spans="1:9">
       <c r="A115" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B115" t="s">
-        <v>24</v>
+        <v>78</v>
       </c>
       <c r="C115" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E115">
-        <v>3574</v>
+        <v>3757</v>
       </c>
       <c r="F115" t="s">
         <v>13</v>
       </c>
       <c r="G115" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="H115" t="s">
         <v>15</v>
@@ -3736,241 +3724,241 @@
     </row>
     <row r="116" spans="1:9">
       <c r="A116" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B116" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C116" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D116" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E116">
-        <v>3665</v>
+        <v>3848</v>
       </c>
       <c r="F116" t="s">
         <v>13</v>
       </c>
       <c r="G116" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H116" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="I116"/>
     </row>
     <row r="117" spans="1:9">
       <c r="A117" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B117" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C117" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D117" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="E117">
-        <v>3727</v>
+        <v>3878</v>
       </c>
       <c r="F117" t="s">
         <v>13</v>
       </c>
       <c r="G117" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="H117" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I117"/>
     </row>
     <row r="118" spans="1:9">
       <c r="A118" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B118" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C118" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D118" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E118">
-        <v>1640</v>
+        <v>3789</v>
       </c>
       <c r="F118" t="s">
         <v>13</v>
       </c>
       <c r="G118" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="H118" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I118"/>
     </row>
     <row r="119" spans="1:9">
       <c r="A119" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B119" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C119" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D119" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E119">
-        <v>3605</v>
+        <v>3909</v>
       </c>
       <c r="F119" t="s">
         <v>13</v>
       </c>
       <c r="G119" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H119" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I119"/>
     </row>
     <row r="120" spans="1:9">
       <c r="A120" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B120" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C120" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D120" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E120">
-        <v>3635</v>
+        <v>3820</v>
       </c>
       <c r="F120" t="s">
         <v>13</v>
       </c>
       <c r="G120" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H120" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I120"/>
     </row>
     <row r="121" spans="1:9">
       <c r="A121" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B121" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="C121" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D121" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E121">
-        <v>3757</v>
+        <v>3941</v>
       </c>
       <c r="F121" t="s">
         <v>13</v>
       </c>
       <c r="G121" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H121" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="I121"/>
     </row>
     <row r="122" spans="1:9">
       <c r="A122" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B122" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C122" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D122" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E122">
-        <v>3848</v>
+        <v>4002</v>
       </c>
       <c r="F122" t="s">
         <v>13</v>
       </c>
       <c r="G122" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H122" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="I122"/>
     </row>
     <row r="123" spans="1:9">
       <c r="A123" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B123" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C123" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" t="s">
         <v>26</v>
       </c>
-      <c r="D123" t="s">
-        <v>21</v>
-      </c>
       <c r="E123">
-        <v>3878</v>
+        <v>4061</v>
       </c>
       <c r="F123" t="s">
         <v>13</v>
       </c>
       <c r="G123" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H123" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I123"/>
     </row>
     <row r="124" spans="1:9">
       <c r="A124" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B124" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C124" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D124" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E124">
-        <v>3789</v>
+        <v>4122</v>
       </c>
       <c r="F124" t="s">
         <v>13</v>
       </c>
       <c r="G124" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H124" t="s">
         <v>15</v>
@@ -3979,246 +3967,84 @@
     </row>
     <row r="125" spans="1:9">
       <c r="A125" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B125" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C125" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D125" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="E125">
-        <v>3909</v>
+        <v>4031</v>
       </c>
       <c r="F125" t="s">
         <v>13</v>
       </c>
       <c r="G125" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="H125" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I125"/>
     </row>
     <row r="126" spans="1:9">
       <c r="A126" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B126" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C126" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D126" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E126">
-        <v>3820</v>
+        <v>4092</v>
       </c>
       <c r="F126" t="s">
         <v>13</v>
       </c>
       <c r="G126" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H126" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I126"/>
     </row>
     <row r="127" spans="1:9">
       <c r="A127" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B127" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C127" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D127" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="E127">
-        <v>3941</v>
+        <v>3972</v>
       </c>
       <c r="F127" t="s">
         <v>13</v>
       </c>
       <c r="G127" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="H127" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="I127"/>
-    </row>
-    <row r="128" spans="1:9">
-      <c r="A128" t="s">
-        <v>84</v>
-      </c>
-      <c r="B128" t="s">
-        <v>20</v>
-      </c>
-      <c r="C128" t="s">
-        <v>25</v>
-      </c>
-      <c r="D128" t="s">
-        <v>34</v>
-      </c>
-      <c r="E128">
-        <v>4002</v>
-      </c>
-      <c r="F128" t="s">
-        <v>13</v>
-      </c>
-      <c r="G128" t="s">
-        <v>27</v>
-      </c>
-      <c r="H128" t="s">
-        <v>15</v>
-      </c>
-      <c r="I128"/>
-    </row>
-    <row r="129" spans="1:9">
-      <c r="A129" t="s">
-        <v>84</v>
-      </c>
-      <c r="B129" t="s">
-        <v>20</v>
-      </c>
-      <c r="C129" t="s">
-        <v>21</v>
-      </c>
-      <c r="D129" t="s">
-        <v>29</v>
-      </c>
-      <c r="E129">
-        <v>4061</v>
-      </c>
-      <c r="F129" t="s">
-        <v>13</v>
-      </c>
-      <c r="G129" t="s">
-        <v>23</v>
-      </c>
-      <c r="H129" t="s">
-        <v>15</v>
-      </c>
-      <c r="I129"/>
-    </row>
-    <row r="130" spans="1:9">
-      <c r="A130" t="s">
-        <v>84</v>
-      </c>
-      <c r="B130" t="s">
-        <v>20</v>
-      </c>
-      <c r="C130" t="s">
-        <v>12</v>
-      </c>
-      <c r="D130" t="s">
-        <v>18</v>
-      </c>
-      <c r="E130">
-        <v>4122</v>
-      </c>
-      <c r="F130" t="s">
-        <v>13</v>
-      </c>
-      <c r="G130" t="s">
-        <v>37</v>
-      </c>
-      <c r="H130" t="s">
-        <v>38</v>
-      </c>
-      <c r="I130"/>
-    </row>
-    <row r="131" spans="1:9">
-      <c r="A131" t="s">
-        <v>84</v>
-      </c>
-      <c r="B131" t="s">
-        <v>20</v>
-      </c>
-      <c r="C131" t="s">
-        <v>28</v>
-      </c>
-      <c r="D131" t="s">
-        <v>26</v>
-      </c>
-      <c r="E131">
-        <v>4031</v>
-      </c>
-      <c r="F131" t="s">
-        <v>13</v>
-      </c>
-      <c r="G131" t="s">
-        <v>30</v>
-      </c>
-      <c r="H131" t="s">
-        <v>15</v>
-      </c>
-      <c r="I131"/>
-    </row>
-    <row r="132" spans="1:9">
-      <c r="A132" t="s">
-        <v>84</v>
-      </c>
-      <c r="B132" t="s">
-        <v>20</v>
-      </c>
-      <c r="C132" t="s">
-        <v>11</v>
-      </c>
-      <c r="D132" t="s">
-        <v>22</v>
-      </c>
-      <c r="E132">
-        <v>4092</v>
-      </c>
-      <c r="F132" t="s">
-        <v>13</v>
-      </c>
-      <c r="G132" t="s">
-        <v>14</v>
-      </c>
-      <c r="H132" t="s">
-        <v>15</v>
-      </c>
-      <c r="I132"/>
-    </row>
-    <row r="133" spans="1:9">
-      <c r="A133" t="s">
-        <v>84</v>
-      </c>
-      <c r="B133" t="s">
-        <v>20</v>
-      </c>
-      <c r="C133" t="s">
-        <v>33</v>
-      </c>
-      <c r="D133" t="s">
-        <v>17</v>
-      </c>
-      <c r="E133">
-        <v>3972</v>
-      </c>
-      <c r="F133" t="s">
-        <v>13</v>
-      </c>
-      <c r="G133" t="s">
-        <v>35</v>
-      </c>
-      <c r="H133" t="s">
-        <v>15</v>
-      </c>
-      <c r="I133"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>